<commit_message>
pruning/filtering based on ontology terms controlled vocabulary
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdeck/IdeaProjects/FutresAPI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A0FE3330-B542-4C4A-A7FB-4B8FE1F9E857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7222E0FC-0542-D24E-8933-07E1A16DD775}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="40">
   <si>
     <t>materialSampleID</t>
   </si>
@@ -133,17 +133,20 @@
     <t>clean</t>
   </si>
   <si>
-    <t>weight</t>
-  </si>
-  <si>
     <t>lb</t>
+  </si>
+  <si>
+    <t>bad value</t>
+  </si>
+  <si>
+    <t>body length with tail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -277,6 +280,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF008000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -620,9 +629,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -977,11 +987,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1091,11 +1101,17 @@
       <c r="O2" t="s">
         <v>24</v>
       </c>
+      <c r="P2">
+        <v>47</v>
+      </c>
+      <c r="Q2">
+        <v>-123</v>
+      </c>
       <c r="R2">
         <v>314</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1124,10 +1140,10 @@
         <v>17</v>
       </c>
       <c r="J3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" t="s">
         <v>37</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="L3">
         <v>27.9</v>
@@ -1137,6 +1153,12 @@
       </c>
       <c r="O3" t="s">
         <v>24</v>
+      </c>
+      <c r="P3">
+        <v>4.1230000000000002</v>
+      </c>
+      <c r="Q3">
+        <v>-123.5</v>
       </c>
       <c r="R3">
         <v>314</v>
@@ -1147,7 +1169,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -1174,7 +1196,7 @@
         <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="L4">
         <v>51.4</v>
@@ -1184,6 +1206,12 @@
       </c>
       <c r="O4" t="s">
         <v>24</v>
+      </c>
+      <c r="P4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>19</v>
       </c>
       <c r="R4">
         <v>314</v>
@@ -1374,6 +1402,53 @@
         <v>24</v>
       </c>
       <c r="R8">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <v>2009</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="1">
+        <v>100</v>
+      </c>
+      <c r="N9" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" t="s">
+        <v>24</v>
+      </c>
+      <c r="R9">
         <v>314</v>
       </c>
     </row>

</xml_diff>